<commit_message>
Done testcase 5-7 in Testcase report
</commit_message>
<xml_diff>
--- a/BTO_Test_Cases.xlsx
+++ b/BTO_Test_Cases.xlsx
@@ -5,22 +5,35 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyna\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a1b14f6b97de3626/Documents/GitHub/SC2002-BTO-System/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6055F1-CD6A-4406-A5A4-040A6CA6974F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{CE6055F1-CD6A-4406-A5A4-040A6CA6974F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E65BA193-BD6E-4BA0-9331-F5922AC70D81}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="105">
   <si>
     <t>Test Case Description</t>
   </si>
@@ -41,9 +54,6 @@
   </si>
   <si>
     <t>Password Change Functionality</t>
-  </si>
-  <si>
-    <t>Project Visibility Based on User Group and Toggle</t>
   </si>
   <si>
     <t>Project Application</t>
@@ -534,6 +544,72 @@
 5
 5. Enter the BTO Name: 
 Tampines Grove</t>
+  </si>
+  <si>
+    <t>Ineligible applicant. No projects available.</t>
+  </si>
+  <si>
+    <t>Project Application
+(U)</t>
+  </si>
+  <si>
+    <t>Project Visibility Based on User Group and Toggle
+User aged &lt; 35 and Single: 
+Not eligible</t>
+  </si>
+  <si>
+    <t>1. Login as Applicant: Tom
+2. Enter NRIC: T1213151J
+3. Enter Pasword: password1
+4. Enter 1 for Projects
+5. Enter 1 to view list of projects</t>
+  </si>
+  <si>
+    <t>1. Login as Applicant: Jane
+2. Enter NRIC: T3344556R
+3. Enter Pasword: password1
+4. Enter 1 for Projects
+5. Enter 1 to view list of projects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+=== Project Details ===
+Name: Bedok Bayshore Drive
+Neighborhood: Bedok
+2-room Units: 100 (Price: $132000.00)
+Application Period: 01-08-2025 to 01-08-2026
+Manager: T4455667S
+Officers: 0/10
+Visibility: Visible to applicants</t>
+  </si>
+  <si>
+    <t>Project Visibility Based on User Group and Toggle
+User aged &gt;= 35 and Single: 
+Only eligible for 2 room</t>
+  </si>
+  <si>
+    <t>Project Visibility Based on User Group and Toggle
+User aged &gt; = 21 and Married: 
+Only eligible for 2 room</t>
+  </si>
+  <si>
+    <t>1. Login as Applicant: Ray
+2. Enter NRIC: T1122334K
+3. Enter Pasword: password1
+4. Enter 1 for Projects
+5. Enter 1 to view list of projects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+=== Project Details ===
+Name: Bedok Bayshore Drive
+Neighborhood: Bedok
+2-room Units: 100 (Price: $132000.00)
+3-room Units: 70 (Price: $310000.00)
+Application Period: 01-08-2025 to 01-08-2026
+Manager: T4455667S
+Officers: 0/10
+Visibility: Visible to applicants</t>
   </si>
 </sst>
 </file>
@@ -621,7 +697,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -629,6 +705,142 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -679,142 +891,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -829,17 +905,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C42C02ED-F60E-45E4-9C8B-B7F52CA76837}" name="Table1" displayName="Table1" ref="A1:H26" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:H26" xr:uid="{C42C02ED-F60E-45E4-9C8B-B7F52CA76837}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C42C02ED-F60E-45E4-9C8B-B7F52CA76837}" name="Table1" displayName="Table1" ref="A1:H29" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H29" xr:uid="{C42C02ED-F60E-45E4-9C8B-B7F52CA76837}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{114D3AF0-17B9-4419-9126-5E81FC8D3CAF}" name="Test Case ID" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{456F26C0-8991-44F8-876A-C515C080C7A3}" name="Test Case Description" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{2C6FD98F-A000-412A-8661-6160F5448948}" name="Expected Behavior" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{3E6A920F-805B-4B1A-BB42-2D45F391DEBC}" name="Failure Indicators" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{044C3883-F7F4-4E27-AAD9-D75CD3C4AA61}" name="Steps" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{0F5F8A6C-613E-4370-A417-B85E0CADF329}" name="Expected Output" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{853B8C11-A801-4E3F-8C15-813C911C910E}" name="Actual Output" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{5CF3F42F-A583-4B55-8990-9CB29434AC24}" name="Status" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{114D3AF0-17B9-4419-9126-5E81FC8D3CAF}" name="Test Case ID" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{456F26C0-8991-44F8-876A-C515C080C7A3}" name="Test Case Description" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{2C6FD98F-A000-412A-8661-6160F5448948}" name="Expected Behavior" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{3E6A920F-805B-4B1A-BB42-2D45F391DEBC}" name="Failure Indicators" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{044C3883-F7F4-4E27-AAD9-D75CD3C4AA61}" name="Steps" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{0F5F8A6C-613E-4370-A417-B85E0CADF329}" name="Expected Output" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{853B8C11-A801-4E3F-8C15-813C911C910E}" name="Actual Output" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{5CF3F42F-A583-4B55-8990-9CB29434AC24}" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1132,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1151,7 +1227,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1163,16 +1239,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -1183,22 +1259,22 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="G2" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="62" x14ac:dyDescent="0.35">
@@ -1209,22 +1285,22 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="77.5" x14ac:dyDescent="0.35">
@@ -1235,22 +1311,22 @@
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="124" x14ac:dyDescent="0.35">
@@ -1261,126 +1337,146 @@
         <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="155" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
+      <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="E9" s="3"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
+      <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="E10" s="3"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
+      <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1388,17 +1484,15 @@
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
+      <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1406,35 +1500,31 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
+      <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A14" s="3">
-        <v>13</v>
-      </c>
+    <row r="14" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1442,35 +1532,31 @@
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A15" s="3">
-        <v>14</v>
-      </c>
+      <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
+    <row r="16" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+      <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1478,169 +1564,155 @@
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A17" s="3">
-        <v>16</v>
-      </c>
+      <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="356.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
-        <v>17</v>
-      </c>
+    <row r="18" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+      <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="155" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
-        <v>83</v>
+        <v>16</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>94</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>95</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="3">
-        <v>18</v>
-      </c>
+    <row r="21" spans="1:8" ht="356.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A22" s="3">
-        <v>19</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="155" x14ac:dyDescent="0.35">
+      <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E22" s="1"/>
+        <v>89</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A23" s="3">
-        <v>20</v>
-      </c>
+    <row r="23" spans="1:8" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E23" s="1"/>
+        <v>90</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A24" s="3">
-        <v>21</v>
-      </c>
+    <row r="24" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="3">
-        <v>22</v>
-      </c>
+    <row r="25" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+      <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -1648,27 +1720,74 @@
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A26" s="3">
-        <v>23</v>
-      </c>
+      <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
+    <row r="27" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>